<commit_message>
SDM 1 extra page
</commit_message>
<xml_diff>
--- a/data/Result_theo.xlsx
+++ b/data/Result_theo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20412"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14060" activeTab="4"/>
+    <workbookView xWindow="-18100" yWindow="1600" windowWidth="25600" windowHeight="14060" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2674" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2696" uniqueCount="302">
   <si>
     <t>Month</t>
   </si>
@@ -927,6 +927,9 @@
   <si>
     <t>ww.lanacion.cl</t>
   </si>
+  <si>
+    <t>sstat keyword</t>
+  </si>
 </sst>
 </file>
 
@@ -990,8 +993,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="127">
+  <cellStyleXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1130,19 +1135,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="127">
+  <cellStyles count="129">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1206,6 +1211,7 @@
     <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1269,6 +1275,7 @@
     <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1521,11 +1528,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2078805672"/>
-        <c:axId val="2075989912"/>
+        <c:axId val="546621464"/>
+        <c:axId val="546915416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2078805672"/>
+        <c:axId val="546621464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1534,7 +1541,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2075989912"/>
+        <c:crossAx val="546915416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1542,7 +1549,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2075989912"/>
+        <c:axId val="546915416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1553,14 +1560,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2078805672"/>
+        <c:crossAx val="546621464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1906,37 +1912,37 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7" t="s">
+      <c r="C1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7" t="s">
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1984,7 +1990,7 @@
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="6">
+      <c r="A3" s="10">
         <v>41275</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -2029,7 +2035,7 @@
       <c r="Q3" s="1"/>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="6"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
@@ -2117,7 +2123,7 @@
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="7"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
@@ -2160,7 +2166,7 @@
       <c r="Q6" s="1"/>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="6">
+      <c r="A7" s="10">
         <v>41699</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -2205,7 +2211,7 @@
       <c r="Q7" s="1"/>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="6"/>
+      <c r="A8" s="10"/>
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
@@ -2248,7 +2254,7 @@
       <c r="Q8" s="1"/>
     </row>
     <row r="9" spans="1:17">
-      <c r="A9" s="6"/>
+      <c r="A9" s="10"/>
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
@@ -2291,7 +2297,7 @@
       <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="1:17">
-      <c r="A10" s="6"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -2379,7 +2385,7 @@
       <c r="Q11" s="1"/>
     </row>
     <row r="12" spans="1:17">
-      <c r="A12" s="7"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
@@ -2422,7 +2428,7 @@
       <c r="Q12" s="1"/>
     </row>
     <row r="13" spans="1:17">
-      <c r="A13" s="7"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2510,7 +2516,7 @@
       <c r="Q14" s="1"/>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" s="7"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
@@ -2553,7 +2559,7 @@
       <c r="Q15" s="1"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="7"/>
+      <c r="A16" s="9"/>
       <c r="B16" s="1" t="s">
         <v>11</v>
       </c>
@@ -2641,7 +2647,7 @@
       <c r="Q17" s="1"/>
     </row>
     <row r="18" spans="1:17">
-      <c r="A18" s="7"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="1" t="s">
         <v>11</v>
       </c>
@@ -2729,7 +2735,7 @@
       <c r="Q19" s="1"/>
     </row>
     <row r="20" spans="1:17">
-      <c r="A20" s="7"/>
+      <c r="A20" s="9"/>
       <c r="B20" s="1" t="s">
         <v>11</v>
       </c>
@@ -2817,7 +2823,7 @@
       <c r="Q21" s="1"/>
     </row>
     <row r="22" spans="1:17">
-      <c r="A22" s="7"/>
+      <c r="A22" s="9"/>
       <c r="B22" s="1" t="s">
         <v>12</v>
       </c>
@@ -2860,7 +2866,7 @@
       <c r="Q22" s="1"/>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="7"/>
+      <c r="A23" s="9"/>
       <c r="B23" s="1" t="s">
         <v>11</v>
       </c>
@@ -2948,7 +2954,7 @@
       <c r="Q24" s="1"/>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" s="7"/>
+      <c r="A25" s="9"/>
       <c r="B25" s="1" t="s">
         <v>12</v>
       </c>
@@ -2991,7 +2997,7 @@
       <c r="Q25" s="1"/>
     </row>
     <row r="26" spans="1:17">
-      <c r="A26" s="7"/>
+      <c r="A26" s="9"/>
       <c r="B26" s="1" t="s">
         <v>11</v>
       </c>
@@ -3034,7 +3040,7 @@
       <c r="Q26" s="1"/>
     </row>
     <row r="27" spans="1:17">
-      <c r="A27" s="6">
+      <c r="A27" s="10">
         <v>41913</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -3079,7 +3085,7 @@
       <c r="Q27" s="1"/>
     </row>
     <row r="28" spans="1:17">
-      <c r="A28" s="7"/>
+      <c r="A28" s="9"/>
       <c r="B28" s="1" t="s">
         <v>12</v>
       </c>
@@ -3122,7 +3128,7 @@
       <c r="Q28" s="1"/>
     </row>
     <row r="29" spans="1:17">
-      <c r="A29" s="7"/>
+      <c r="A29" s="9"/>
       <c r="B29" s="1" t="s">
         <v>11</v>
       </c>
@@ -3210,7 +3216,7 @@
       <c r="Q30" s="1"/>
     </row>
     <row r="31" spans="1:17">
-      <c r="A31" s="7"/>
+      <c r="A31" s="9"/>
       <c r="B31" s="1" t="s">
         <v>12</v>
       </c>
@@ -3253,7 +3259,7 @@
       <c r="Q31" s="1"/>
     </row>
     <row r="32" spans="1:17">
-      <c r="A32" s="7"/>
+      <c r="A32" s="9"/>
       <c r="B32" s="1" t="s">
         <v>11</v>
       </c>
@@ -3341,7 +3347,7 @@
       <c r="Q33" s="1"/>
     </row>
     <row r="34" spans="1:17">
-      <c r="A34" s="7"/>
+      <c r="A34" s="9"/>
       <c r="B34" s="1" t="s">
         <v>12</v>
       </c>
@@ -3384,7 +3390,7 @@
       <c r="Q34" s="1"/>
     </row>
     <row r="35" spans="1:17">
-      <c r="A35" s="7"/>
+      <c r="A35" s="9"/>
       <c r="B35" s="1" t="s">
         <v>11</v>
       </c>
@@ -3472,7 +3478,7 @@
       <c r="Q36" s="1"/>
     </row>
     <row r="37" spans="1:17">
-      <c r="A37" s="7"/>
+      <c r="A37" s="9"/>
       <c r="B37" s="1" t="s">
         <v>11</v>
       </c>
@@ -3734,7 +3740,7 @@
       <c r="Q42" s="1"/>
     </row>
     <row r="43" spans="1:17">
-      <c r="A43" s="7"/>
+      <c r="A43" s="9"/>
       <c r="B43" s="1" t="s">
         <v>12</v>
       </c>
@@ -3777,7 +3783,7 @@
       <c r="Q43" s="1"/>
     </row>
     <row r="44" spans="1:17">
-      <c r="A44" s="7"/>
+      <c r="A44" s="9"/>
       <c r="B44" s="1" t="s">
         <v>11</v>
       </c>
@@ -7880,6 +7886,17 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A17:A18"/>
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="A38:A41"/>
     <mergeCell ref="A42:A44"/>
@@ -7889,17 +7906,6 @@
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="A30:A32"/>
     <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="M1:Q1"/>
-    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -35850,7 +35856,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -35862,15 +35867,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:R42"/>
+  <dimension ref="B1:X42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B15"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="V25" sqref="V25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="19" max="19" width="13" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:11">
+    <row r="1" spans="2:24">
       <c r="B1" s="5">
         <v>41652</v>
       </c>
@@ -35901,8 +35909,20 @@
       <c r="K1">
         <v>0.53</v>
       </c>
-    </row>
-    <row r="2" spans="2:11">
+      <c r="L1">
+        <v>0.67</v>
+      </c>
+      <c r="M1">
+        <v>0.33</v>
+      </c>
+      <c r="N1">
+        <v>0.44220000000000004</v>
+      </c>
+      <c r="S1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="2" spans="2:24">
       <c r="B2" s="5">
         <v>41683</v>
       </c>
@@ -35933,8 +35953,26 @@
       <c r="K2">
         <v>0.67</v>
       </c>
-    </row>
-    <row r="3" spans="2:11">
+      <c r="L2">
+        <v>0.67</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>0.80239520958083832</v>
+      </c>
+      <c r="S2" t="s">
+        <v>62</v>
+      </c>
+      <c r="U2" t="s">
+        <v>63</v>
+      </c>
+      <c r="W2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="2:24">
       <c r="B3" s="5">
         <v>41711</v>
       </c>
@@ -35965,8 +36003,38 @@
       <c r="K3">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="4" spans="2:11">
+      <c r="L3">
+        <v>0.6</v>
+      </c>
+      <c r="M3">
+        <v>0.75</v>
+      </c>
+      <c r="N3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="S3">
+        <f>L1-I1</f>
+        <v>0.23000000000000004</v>
+      </c>
+      <c r="T3">
+        <v>14</v>
+      </c>
+      <c r="U3">
+        <f>J1-M1</f>
+        <v>0.34</v>
+      </c>
+      <c r="V3">
+        <v>8</v>
+      </c>
+      <c r="W3">
+        <f>K1-N1</f>
+        <v>8.7799999999999989E-2</v>
+      </c>
+      <c r="X3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:24">
       <c r="B4" s="5">
         <v>41742</v>
       </c>
@@ -35997,8 +36065,35 @@
       <c r="K4">
         <v>0.73</v>
       </c>
-    </row>
-    <row r="5" spans="2:11">
+      <c r="L4">
+        <v>0.33</v>
+      </c>
+      <c r="M4">
+        <v>0.25</v>
+      </c>
+      <c r="N4">
+        <v>0.28448275862068967</v>
+      </c>
+      <c r="S4">
+        <f t="shared" ref="S4:S19" si="0">L2-I2</f>
+        <v>0.17000000000000004</v>
+      </c>
+      <c r="T4">
+        <v>13</v>
+      </c>
+      <c r="U4">
+        <f t="shared" ref="U4:U17" si="1">J2-M2</f>
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <f t="shared" ref="W4:W17" si="2">K2-N2</f>
+        <v>-0.13239520958083828</v>
+      </c>
+      <c r="X4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:24">
       <c r="B5" s="5">
         <v>41772</v>
       </c>
@@ -36029,8 +36124,38 @@
       <c r="K5">
         <v>0.47</v>
       </c>
-    </row>
-    <row r="6" spans="2:11">
+      <c r="L5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M5">
+        <v>0.4</v>
+      </c>
+      <c r="N5">
+        <v>0.336231884057971</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="T5">
+        <v>11</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="1"/>
+        <v>-0.25</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="2"/>
+        <v>-0.16666666666666663</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:24">
       <c r="B6" s="5">
         <v>41803</v>
       </c>
@@ -36061,8 +36186,35 @@
       <c r="K6">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="7" spans="2:11">
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="0"/>
+        <v>-0.23999999999999994</v>
+      </c>
+      <c r="T6">
+        <v>4.5</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="2"/>
+        <v>0.44551724137931031</v>
+      </c>
+      <c r="X6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:24">
       <c r="B7" s="5">
         <v>41833</v>
       </c>
@@ -36093,8 +36245,38 @@
       <c r="K7">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="8" spans="2:11">
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="0"/>
+        <v>-9.0000000000000024E-2</v>
+      </c>
+      <c r="T7">
+        <v>8</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="1"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="V7">
+        <v>3.5</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="2"/>
+        <v>0.13376811594202898</v>
+      </c>
+      <c r="X7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:24">
       <c r="B8" s="5">
         <v>41864</v>
       </c>
@@ -36125,8 +36307,38 @@
       <c r="K8">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="9" spans="2:11">
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="0"/>
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="T8">
+        <v>7</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="V8">
+        <v>11</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="X8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:24">
       <c r="B9" s="5">
         <v>41895</v>
       </c>
@@ -36157,8 +36369,38 @@
       <c r="K9">
         <v>0.67</v>
       </c>
-    </row>
-    <row r="10" spans="2:11">
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="0"/>
+        <v>-0.2</v>
+      </c>
+      <c r="T9">
+        <v>6</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="V9">
+        <v>11</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="2"/>
+        <v>0.33</v>
+      </c>
+      <c r="X9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="2:24">
       <c r="B10" s="5">
         <v>41925</v>
       </c>
@@ -36189,8 +36431,38 @@
       <c r="K10">
         <v>0.47</v>
       </c>
-    </row>
-    <row r="11" spans="2:11">
+      <c r="L10">
+        <v>0.5</v>
+      </c>
+      <c r="M10">
+        <v>0.4</v>
+      </c>
+      <c r="N10">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="0"/>
+        <v>-0.67</v>
+      </c>
+      <c r="T10">
+        <v>1.5</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="V10">
+        <v>11</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="2"/>
+        <v>0.8</v>
+      </c>
+      <c r="X10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="2:24">
       <c r="B11" s="5">
         <v>41956</v>
       </c>
@@ -36221,8 +36493,38 @@
       <c r="K11">
         <v>0.57999999999999996</v>
       </c>
-    </row>
-    <row r="12" spans="2:11">
+      <c r="L11">
+        <v>0.75</v>
+      </c>
+      <c r="M11">
+        <v>0.5</v>
+      </c>
+      <c r="N11">
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="0"/>
+        <v>-0.67</v>
+      </c>
+      <c r="T11">
+        <v>1.5</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="1"/>
+        <v>0.67</v>
+      </c>
+      <c r="V11">
+        <v>9</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="2"/>
+        <v>0.67</v>
+      </c>
+      <c r="X11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:24">
       <c r="B12" s="5">
         <v>41986</v>
       </c>
@@ -36253,8 +36555,38 @@
       <c r="K12">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="13" spans="2:11">
+      <c r="L12">
+        <v>0.75</v>
+      </c>
+      <c r="M12">
+        <v>0.27</v>
+      </c>
+      <c r="N12">
+        <v>0.3970588235294118</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="0"/>
+        <v>0.12</v>
+      </c>
+      <c r="T12">
+        <v>12</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="1"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="V12">
+        <v>3.5</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="2"/>
+        <v>2.5555555555555554E-2</v>
+      </c>
+      <c r="X12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:24">
       <c r="B13" s="5">
         <v>41653</v>
       </c>
@@ -36285,8 +36617,38 @@
       <c r="K13">
         <v>0.67</v>
       </c>
-    </row>
-    <row r="14" spans="2:11">
+      <c r="L13">
+        <v>0.43</v>
+      </c>
+      <c r="M13">
+        <v>0.38</v>
+      </c>
+      <c r="N13">
+        <v>0.40345679012345675</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="T13">
+        <v>15</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="1"/>
+        <v>0.32999999999999996</v>
+      </c>
+      <c r="V13">
+        <v>7</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="2"/>
+        <v>-2.0000000000000129E-2</v>
+      </c>
+      <c r="X13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:24">
       <c r="B14" s="5">
         <v>41684</v>
       </c>
@@ -36317,8 +36679,38 @@
       <c r="K14">
         <v>0.67</v>
       </c>
-    </row>
-    <row r="15" spans="2:11">
+      <c r="L14">
+        <v>0.43</v>
+      </c>
+      <c r="M14">
+        <v>0.5</v>
+      </c>
+      <c r="N14">
+        <v>0.46236559139784938</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="0"/>
+        <v>7.999999999999996E-2</v>
+      </c>
+      <c r="T14">
+        <v>10</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="1"/>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="V14">
+        <v>6</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="2"/>
+        <v>0.20294117647058818</v>
+      </c>
+      <c r="X14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:24">
       <c r="B15" s="5">
         <v>41712</v>
       </c>
@@ -36350,16 +36742,87 @@
         <f>2*J15*I15/(I15+J15)</f>
         <v>0.61538461538461542</v>
       </c>
-    </row>
-    <row r="17" spans="4:18">
+      <c r="L15">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="M15">
+        <v>0.8</v>
+      </c>
+      <c r="N15">
+        <v>0.66569343065693432</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="0"/>
+        <v>-0.27999999999999997</v>
+      </c>
+      <c r="T15">
+        <v>3</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="V15">
+        <v>5</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="2"/>
+        <v>0.26654320987654329</v>
+      </c>
+      <c r="X15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="2:24">
+      <c r="S16">
+        <f>L14-I14</f>
+        <v>-0.24000000000000005</v>
+      </c>
+      <c r="T16">
+        <v>4.5</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="1"/>
+        <v>0.17000000000000004</v>
+      </c>
+      <c r="V16">
+        <v>2</v>
+      </c>
+      <c r="W16">
+        <f t="shared" si="2"/>
+        <v>0.20763440860215066</v>
+      </c>
+      <c r="X16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="4:24">
       <c r="D17" t="s">
         <v>65</v>
       </c>
       <c r="M17" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="18" spans="4:18">
+      <c r="S17">
+        <f t="shared" si="0"/>
+        <v>6.9999999999999951E-2</v>
+      </c>
+      <c r="T17">
+        <v>9</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <f t="shared" si="2"/>
+        <v>-5.0308815272318896E-2</v>
+      </c>
+      <c r="X17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="4:24">
       <c r="D18" t="s">
         <v>62</v>
       </c>
@@ -36379,7 +36842,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="4:18">
+    <row r="19" spans="4:24">
       <c r="D19">
         <f>I1-C1</f>
         <v>-0.06</v>
@@ -36388,21 +36851,21 @@
         <v>4.5</v>
       </c>
       <c r="F19">
-        <f>J1-D1</f>
+        <f t="shared" ref="F19:F33" si="3">J1-D1</f>
         <v>0.5</v>
       </c>
       <c r="G19">
         <v>15</v>
       </c>
       <c r="H19">
-        <f>K1-E1</f>
+        <f t="shared" ref="H19:H33" si="4">K1-E1</f>
         <v>0.28000000000000003</v>
       </c>
       <c r="I19">
         <v>12.5</v>
       </c>
       <c r="M19">
-        <f>I1-F1</f>
+        <f t="shared" ref="M19:M33" si="5">I1-F1</f>
         <v>0.31</v>
       </c>
       <c r="N19">
@@ -36419,543 +36882,654 @@
       <c r="R19">
         <v>10.5</v>
       </c>
-    </row>
-    <row r="20" spans="4:18">
+      <c r="S19" t="s">
+        <v>59</v>
+      </c>
+      <c r="T19">
+        <f>T3+T4+T5+T12+T13+T14+T17</f>
+        <v>84</v>
+      </c>
+      <c r="U19" t="s">
+        <v>59</v>
+      </c>
+      <c r="V19">
+        <f>V3+V7+V8+V9+V10+V11+V12+V14+V13+V15+V16</f>
+        <v>77</v>
+      </c>
+      <c r="W19" t="s">
+        <v>59</v>
+      </c>
+      <c r="X19">
+        <f>X3+X6+X7+X8+X9+X10+X11+X12+X14+X15+X16</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="4:24">
       <c r="D20">
-        <f t="shared" ref="D20:D34" si="0">I2-C2</f>
+        <f t="shared" ref="D20:D33" si="6">I2-C2</f>
         <v>-2.0000000000000018E-2</v>
       </c>
       <c r="E20">
         <v>1.5</v>
       </c>
       <c r="F20">
-        <f>J2-D2</f>
+        <f t="shared" si="3"/>
         <v>0.21999999999999997</v>
       </c>
       <c r="G20">
         <v>6</v>
       </c>
       <c r="H20">
-        <f>K2-E2</f>
+        <f t="shared" si="4"/>
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="I20">
         <v>4</v>
       </c>
       <c r="M20">
-        <f>I2-F2</f>
+        <f t="shared" si="5"/>
         <v>0.38</v>
       </c>
       <c r="N20">
         <v>10</v>
       </c>
       <c r="O20">
-        <f t="shared" ref="O20:O33" si="1">J2-G2</f>
+        <f t="shared" ref="O20:O33" si="7">J2-G2</f>
         <v>0</v>
       </c>
       <c r="Q20">
-        <f t="shared" ref="Q20:Q33" si="2">K2-H2</f>
+        <f t="shared" ref="Q20:Q33" si="8">K2-H2</f>
         <v>0.46000000000000008</v>
       </c>
       <c r="R20">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="4:18">
+      <c r="S20" t="s">
+        <v>60</v>
+      </c>
+      <c r="T20">
+        <f>T6+T7+T8+T9+T10+T11+T15+T16</f>
+        <v>36</v>
+      </c>
+      <c r="U20" t="s">
+        <v>60</v>
+      </c>
+      <c r="V20">
+        <f>V5</f>
+        <v>1</v>
+      </c>
+      <c r="W20" t="s">
+        <v>60</v>
+      </c>
+      <c r="X20">
+        <f>X4+X5+X13+X17</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="4:24">
       <c r="D21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>-0.19999999999999996</v>
       </c>
       <c r="E21">
         <v>10</v>
       </c>
       <c r="F21">
-        <f>J3-D3</f>
+        <f t="shared" si="3"/>
         <v>0.15000000000000002</v>
       </c>
       <c r="G21">
         <v>5</v>
       </c>
       <c r="H21">
-        <f>K3-E3</f>
+        <f t="shared" si="4"/>
         <v>3.999999999999998E-2</v>
       </c>
       <c r="I21">
         <v>3</v>
       </c>
       <c r="M21">
-        <f>I3-F3</f>
+        <f t="shared" si="5"/>
         <v>0.21000000000000002</v>
       </c>
       <c r="N21">
         <v>5.5</v>
       </c>
       <c r="O21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.13</v>
       </c>
       <c r="R21">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="4:18">
+    <row r="22" spans="4:24">
       <c r="D22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>-0.21000000000000008</v>
       </c>
       <c r="E22">
         <v>11</v>
       </c>
       <c r="F22">
-        <f>J4-D4</f>
+        <f t="shared" si="3"/>
         <v>0.41000000000000003</v>
       </c>
       <c r="G22">
         <v>14</v>
       </c>
       <c r="H22">
-        <f>K4-E4</f>
+        <f t="shared" si="4"/>
         <v>5.9999999999999942E-2</v>
       </c>
       <c r="I22">
         <v>5</v>
       </c>
       <c r="M22">
-        <f>I4-F4</f>
+        <f t="shared" si="5"/>
         <v>-3.0000000000000027E-2</v>
       </c>
       <c r="N22">
         <v>1</v>
       </c>
       <c r="O22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0.25</v>
       </c>
       <c r="P22">
         <v>3</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>5.9999999999999942E-2</v>
       </c>
       <c r="R22">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="4:18">
+      <c r="S22" t="s">
+        <v>67</v>
+      </c>
+      <c r="T22">
+        <v>36</v>
+      </c>
+      <c r="U22" t="s">
+        <v>67</v>
+      </c>
+      <c r="V22">
+        <v>1</v>
+      </c>
+      <c r="W22" t="s">
+        <v>67</v>
+      </c>
+      <c r="X22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="4:24">
       <c r="D23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>-0.13</v>
       </c>
       <c r="E23">
         <v>8</v>
       </c>
       <c r="F23">
-        <f>J5-D5</f>
+        <f t="shared" si="3"/>
         <v>0.12</v>
       </c>
       <c r="G23">
         <v>3</v>
       </c>
       <c r="H23">
-        <f>K5-E5</f>
+        <f t="shared" si="4"/>
         <v>-7.0000000000000062E-2</v>
       </c>
       <c r="I23">
         <v>7</v>
       </c>
       <c r="M23">
-        <f>I5-F5</f>
+        <f t="shared" si="5"/>
         <v>0.24</v>
       </c>
       <c r="N23">
         <v>7.5</v>
       </c>
       <c r="O23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0.39999999999999997</v>
       </c>
       <c r="P23">
         <v>5</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.30999999999999994</v>
       </c>
       <c r="R23">
         <v>10.5</v>
       </c>
-    </row>
-    <row r="24" spans="4:18">
+      <c r="S23" t="s">
+        <v>70</v>
+      </c>
+      <c r="T23">
+        <f>T19-T20</f>
+        <v>48</v>
+      </c>
+      <c r="U23" t="s">
+        <v>71</v>
+      </c>
+      <c r="V23">
+        <f>V19-V20</f>
+        <v>76</v>
+      </c>
+      <c r="W23" t="s">
+        <v>70</v>
+      </c>
+      <c r="X23">
+        <f>X19-X20</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="4:24">
       <c r="D24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>-7.9999999999999988E-2</v>
       </c>
       <c r="E24">
         <v>6</v>
       </c>
       <c r="F24">
-        <f>J6-D6</f>
+        <f t="shared" si="3"/>
         <v>0.31999999999999995</v>
       </c>
       <c r="G24">
         <v>8.5</v>
       </c>
       <c r="H24">
-        <f>K6-E6</f>
+        <f t="shared" si="4"/>
         <v>-8.0000000000000016E-2</v>
       </c>
       <c r="I24">
         <v>8</v>
       </c>
       <c r="M24">
-        <f>I6-F6</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="R24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="4:18">
+      <c r="S24" t="s">
+        <v>68</v>
+      </c>
+      <c r="T24">
+        <f>(T23-0.5)/SQRT(15*16*31/6)</f>
+        <v>1.3489093563367789</v>
+      </c>
+      <c r="U24" t="s">
+        <v>68</v>
+      </c>
+      <c r="V24">
+        <f>(V23-0.5)/SQRT(12*13*25/6)</f>
+        <v>2.9613536405865788</v>
+      </c>
+      <c r="W24" t="s">
+        <v>68</v>
+      </c>
+      <c r="X24">
+        <f>(X23-0.5)/SQRT(15*16*31/6)</f>
+        <v>2.8256101253791472</v>
+      </c>
+    </row>
+    <row r="25" spans="4:24">
       <c r="D25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>-1.999999999999999E-2</v>
       </c>
       <c r="E25">
         <v>1.5</v>
       </c>
       <c r="F25">
-        <f>J7-D7</f>
+        <f t="shared" si="3"/>
         <v>0.31999999999999995</v>
       </c>
       <c r="G25">
         <v>8.5</v>
       </c>
       <c r="H25">
-        <f>K7-E7</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M25">
-        <f>I7-F7</f>
+        <f t="shared" si="5"/>
         <v>0.06</v>
       </c>
       <c r="N25">
         <v>2</v>
       </c>
       <c r="O25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>8.0000000000000016E-2</v>
       </c>
       <c r="R25">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="4:18">
+    <row r="26" spans="4:24">
       <c r="D26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0.27</v>
       </c>
       <c r="E26">
         <v>14</v>
       </c>
       <c r="F26">
-        <f>J8-D8</f>
+        <f t="shared" si="3"/>
         <v>0.4</v>
       </c>
       <c r="G26">
         <v>13</v>
       </c>
       <c r="H26">
-        <f>K8-E8</f>
+        <f t="shared" si="4"/>
         <v>0.33000000000000007</v>
       </c>
-      <c r="I26" s="9">
+      <c r="I26" s="6">
         <v>14</v>
       </c>
       <c r="M26">
-        <f>I8-F8</f>
+        <f t="shared" si="5"/>
         <v>0.47000000000000003</v>
       </c>
       <c r="N26">
         <v>13</v>
       </c>
       <c r="O26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.47000000000000003</v>
       </c>
       <c r="R26">
         <v>14</v>
       </c>
-    </row>
-    <row r="27" spans="4:18">
+      <c r="S26" t="s">
+        <v>72</v>
+      </c>
+      <c r="V26" t="s">
+        <v>73</v>
+      </c>
+      <c r="X26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="4:24">
       <c r="D27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0.17000000000000004</v>
       </c>
       <c r="E27">
         <v>8</v>
       </c>
       <c r="F27">
-        <f>J9-D9</f>
+        <f t="shared" si="3"/>
         <v>0.34</v>
       </c>
       <c r="G27">
         <v>10</v>
       </c>
       <c r="H27">
-        <f>K9-E9</f>
+        <f t="shared" si="4"/>
         <v>0.28000000000000003</v>
       </c>
-      <c r="I27" s="9">
+      <c r="I27" s="6">
         <v>12.5</v>
       </c>
       <c r="M27">
-        <f>I9-F9</f>
+        <f t="shared" si="5"/>
         <v>0.44000000000000006</v>
       </c>
       <c r="N27">
         <v>12</v>
       </c>
       <c r="O27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>-0.32999999999999996</v>
       </c>
       <c r="P27">
         <v>4</v>
       </c>
       <c r="Q27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="R27">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="4:18">
+    <row r="28" spans="4:24">
       <c r="D28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>-0.24</v>
       </c>
       <c r="E28">
         <v>13</v>
       </c>
       <c r="F28">
-        <f>J10-D10</f>
+        <f t="shared" si="3"/>
         <v>0.36</v>
       </c>
       <c r="G28">
         <v>11</v>
       </c>
       <c r="H28">
-        <f>K10-E10</f>
+        <f t="shared" si="4"/>
         <v>0.12</v>
       </c>
       <c r="I28">
         <v>10</v>
       </c>
       <c r="M28">
-        <f>I10-F10</f>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="N28">
         <v>3</v>
       </c>
       <c r="O28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>-0.20000000000000007</v>
       </c>
       <c r="P28">
         <v>2</v>
       </c>
       <c r="Q28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1.9999999999999962E-2</v>
       </c>
       <c r="R28">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="4:18">
+    <row r="29" spans="4:24">
       <c r="D29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>-0.44</v>
       </c>
       <c r="E29">
         <v>15</v>
       </c>
       <c r="F29">
-        <f>J11-D11</f>
+        <f t="shared" si="3"/>
         <v>0.38999999999999996</v>
       </c>
       <c r="G29">
         <v>12</v>
       </c>
       <c r="H29">
-        <f>K11-E11</f>
+        <f t="shared" si="4"/>
         <v>-1.0000000000000009E-2</v>
       </c>
       <c r="I29">
         <v>1</v>
       </c>
       <c r="M29">
-        <f>I11-F11</f>
+        <f t="shared" si="5"/>
         <v>0.24000000000000002</v>
       </c>
       <c r="N29">
         <v>7.5</v>
       </c>
       <c r="O29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.23999999999999994</v>
       </c>
       <c r="R29">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="4:18">
+    <row r="30" spans="4:24">
       <c r="D30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>-0.22999999999999998</v>
       </c>
       <c r="E30">
         <v>11</v>
       </c>
       <c r="F30">
-        <f>J12-D12</f>
+        <f t="shared" si="3"/>
         <v>0.23000000000000004</v>
       </c>
       <c r="G30">
         <v>7</v>
       </c>
       <c r="H30">
-        <f>K12-E12</f>
+        <f t="shared" si="4"/>
         <v>0.13</v>
       </c>
       <c r="I30">
         <v>11</v>
       </c>
       <c r="M30">
-        <f>I12-F12</f>
+        <f t="shared" si="5"/>
         <v>-7.999999999999996E-2</v>
       </c>
       <c r="N30">
         <v>4</v>
       </c>
       <c r="O30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>-3.0000000000000027E-2</v>
       </c>
       <c r="R30">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="4:18">
+    <row r="31" spans="4:24">
       <c r="D31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>5.9999999999999942E-2</v>
       </c>
       <c r="E31">
         <v>4.5</v>
       </c>
       <c r="F31">
-        <f>J13-D13</f>
+        <f t="shared" si="3"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="G31">
         <v>4</v>
       </c>
       <c r="H31">
-        <f>K13-E13</f>
+        <f t="shared" si="4"/>
         <v>0.10999999999999999</v>
       </c>
       <c r="I31">
         <v>9</v>
       </c>
       <c r="M31">
-        <f>I13-F13</f>
+        <f t="shared" si="5"/>
         <v>0.52</v>
       </c>
       <c r="N31">
         <v>14</v>
       </c>
       <c r="O31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0.13</v>
       </c>
       <c r="P31">
         <v>1</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.39</v>
       </c>
       <c r="R31">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="4:18">
+    <row r="32" spans="4:24">
       <c r="D32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0.10999999999999999</v>
       </c>
       <c r="E32">
         <v>7</v>
       </c>
       <c r="F32">
-        <f>J14-D14</f>
+        <f t="shared" si="3"/>
         <v>-6.9999999999999951E-2</v>
       </c>
       <c r="G32">
         <v>1</v>
       </c>
       <c r="H32">
-        <f>K14-E14</f>
+        <f t="shared" si="4"/>
         <v>3.0000000000000027E-2</v>
       </c>
       <c r="I32">
         <v>2</v>
       </c>
       <c r="M32">
-        <f>I14-F14</f>
+        <f t="shared" si="5"/>
         <v>0.4</v>
       </c>
       <c r="N32">
         <v>11</v>
       </c>
       <c r="O32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.29000000000000004</v>
       </c>
       <c r="R32">
@@ -36964,39 +37538,39 @@
     </row>
     <row r="33" spans="3:18">
       <c r="D33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>-5.0000000000000044E-2</v>
       </c>
       <c r="E33">
         <v>3</v>
       </c>
       <c r="F33">
-        <f>J15-D15</f>
+        <f t="shared" si="3"/>
         <v>-7.999999999999996E-2</v>
       </c>
       <c r="G33">
         <v>2</v>
       </c>
       <c r="H33">
-        <f>K15-E15</f>
+        <f t="shared" si="4"/>
         <v>-6.461538461538463E-2</v>
       </c>
       <c r="I33">
         <v>6</v>
       </c>
       <c r="M33">
-        <f>I15-F15</f>
+        <f t="shared" si="5"/>
         <v>0.21000000000000002</v>
       </c>
       <c r="N33">
         <v>5.5</v>
       </c>
       <c r="O33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.19538461538461543</v>
       </c>
       <c r="R33">
@@ -37247,7 +37821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="B24" sqref="B24:D38"/>
     </sheetView>
   </sheetViews>
@@ -37270,7 +37844,7 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="10">
+      <c r="A4" s="7">
         <v>41287</v>
       </c>
       <c r="B4">
@@ -37284,7 +37858,7 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="10">
+      <c r="A5" s="7">
         <v>41318</v>
       </c>
       <c r="B5">
@@ -37298,7 +37872,7 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="10">
+      <c r="A6" s="7">
         <v>41346</v>
       </c>
       <c r="B6">
@@ -37312,7 +37886,7 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="10">
+      <c r="A7" s="7">
         <v>41377</v>
       </c>
       <c r="B7">
@@ -37326,7 +37900,7 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="10">
+      <c r="A8" s="7">
         <v>41407</v>
       </c>
       <c r="B8">
@@ -37340,7 +37914,7 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="10">
+      <c r="A9" s="7">
         <v>41438</v>
       </c>
       <c r="B9">
@@ -37354,7 +37928,7 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="10">
+      <c r="A10" s="7">
         <v>41468</v>
       </c>
       <c r="B10">
@@ -37368,7 +37942,7 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="10">
+      <c r="A11" s="7">
         <v>41499</v>
       </c>
       <c r="B11">
@@ -37382,7 +37956,7 @@
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="10">
+      <c r="A12" s="7">
         <v>41530</v>
       </c>
       <c r="B12">
@@ -37396,7 +37970,7 @@
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="10">
+      <c r="A13" s="7">
         <v>41560</v>
       </c>
       <c r="B13">
@@ -37410,7 +37984,7 @@
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="10">
+      <c r="A14" s="7">
         <v>41591</v>
       </c>
       <c r="B14">
@@ -37424,7 +37998,7 @@
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="10">
+      <c r="A15" s="7">
         <v>41621</v>
       </c>
       <c r="B15">
@@ -37438,7 +38012,7 @@
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="10">
+      <c r="A16" s="7">
         <v>41653</v>
       </c>
       <c r="B16">
@@ -37452,7 +38026,7 @@
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="10">
+      <c r="A17" s="7">
         <v>41684</v>
       </c>
       <c r="B17">
@@ -37466,7 +38040,7 @@
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="10">
+      <c r="A18" s="7">
         <v>41712</v>
       </c>
       <c r="B18">
@@ -37707,7 +38281,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -37720,7 +38293,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N273"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="N2" sqref="N2:N27"/>
     </sheetView>
   </sheetViews>
@@ -40657,7 +41230,6 @@
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>